<commit_message>
fixed error name for xml
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel_Ini/Guild.xlsx
+++ b/_Out/NFDataCfg/Excel_Ini/Guild.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cherish\Desktop\git\nf\develop\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27520" windowHeight="17540" activeTab="1"/>
+    <workbookView windowWidth="21495" windowHeight="10342"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -19,27 +14,19 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" refreshedVersion="2" background="1" saveData="1">
-    <webPr xml="1" sourceData="1" parsePre="1" consecutive="1" xl2000="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Skill" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90">
   <si>
     <t>Id</t>
   </si>
@@ -71,10 +58,10 @@
     <t>GuildContinueDay</t>
   </si>
   <si>
-    <t>GuilID</t>
-  </si>
-  <si>
-    <t>GuilIDIcon</t>
+    <t>GuildID</t>
+  </si>
+  <si>
+    <t>GuildIcon</t>
   </si>
   <si>
     <t>GuildMemeberCount</t>
@@ -149,6 +136,9 @@
     <t>Ref</t>
   </si>
   <si>
+    <t>Upload</t>
+  </si>
+  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -306,25 +296,23 @@
   </si>
   <si>
     <t>GuildSkill</t>
-  </si>
-  <si>
-    <t>Upload</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Upload</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+  </numFmts>
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -332,8 +320,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -344,13 +332,151 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,8 +495,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -494,9 +806,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -538,13 +1092,61 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
@@ -558,20 +1160,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2">
     <tableStyle name="MySqlDefault" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -827,37 +1421,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" customWidth="1"/>
+    <col min="1" max="1" width="8.36283185840708" customWidth="1"/>
+    <col min="2" max="2" width="18.3628318584071" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="8.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="8" width="11.6328125" customWidth="1"/>
-    <col min="9" max="9" width="18.36328125" customWidth="1"/>
-    <col min="12" max="12" width="19.36328125" customWidth="1"/>
-    <col min="13" max="13" width="22.6328125" customWidth="1"/>
-    <col min="14" max="14" width="11.6328125" customWidth="1"/>
-    <col min="15" max="15" width="17.1796875" customWidth="1"/>
-    <col min="16" max="16" width="16.1796875" customWidth="1"/>
+    <col min="5" max="5" width="8.45132743362832" customWidth="1"/>
+    <col min="6" max="6" width="10.4513274336283" customWidth="1"/>
+    <col min="7" max="8" width="11.6371681415929" customWidth="1"/>
+    <col min="9" max="9" width="18.3628318584071" customWidth="1"/>
+    <col min="12" max="12" width="19.3628318584071" customWidth="1"/>
+    <col min="13" max="13" width="22.6371681415929" customWidth="1"/>
+    <col min="14" max="14" width="11.6371681415929" customWidth="1"/>
+    <col min="15" max="15" width="17.1769911504425" customWidth="1"/>
+    <col min="16" max="16" width="16.1769911504425" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="4" customFormat="1" spans="1:27">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -940,7 +1535,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="1" spans="1:27">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -1023,7 +1618,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="2" customFormat="1" spans="1:27">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -1106,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" spans="1:27">
       <c r="A4" s="8" t="s">
         <v>32</v>
       </c>
@@ -1189,7 +1784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" s="2" customFormat="1" spans="1:27">
       <c r="A5" s="8" t="s">
         <v>33</v>
       </c>
@@ -1272,7 +1867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" spans="1:27">
       <c r="A6" s="8" t="s">
         <v>34</v>
       </c>
@@ -1355,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="5" customFormat="1" ht="13.5" spans="1:27">
       <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
@@ -1438,9 +2033,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" s="5" customFormat="1" ht="18" customHeight="1" spans="1:27">
       <c r="A8" s="9" t="s">
-        <v>89</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>0</v>
@@ -1521,140 +2116,141 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" s="6" customFormat="1" ht="15" spans="1:27">
       <c r="A9" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O9" s="6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Z9" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA9" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AA8">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:XFD63"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A63" sqref="$A63:$XFD63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="8.72566371681416" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" s="2" customFormat="1" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
@@ -1662,7 +2258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" s="2" customFormat="1" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>32</v>
       </c>
@@ -1670,7 +2266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" spans="1:2">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1678,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" s="2" customFormat="1" spans="1:2">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -1686,41 +2282,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" s="2" customFormat="1" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" s="2" customFormat="1" spans="1:8">
       <c r="A9" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" s="2" customFormat="1" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
@@ -1746,39 +2342,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" s="2" customFormat="1" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" s="2" customFormat="1" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B13" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" s="2" customFormat="1" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" s="2" customFormat="1" spans="1:2">
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
@@ -1786,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" s="2" customFormat="1" spans="1:2">
       <c r="A16" s="2" t="s">
         <v>32</v>
       </c>
@@ -1794,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" s="2" customFormat="1" spans="1:2">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1802,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" s="2" customFormat="1" spans="1:2">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1810,59 +2406,59 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" s="2" customFormat="1" spans="1:2">
       <c r="A19" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" s="2" customFormat="1" spans="1:14">
       <c r="A20" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" s="2" customFormat="1" spans="1:14">
       <c r="A21" s="2" t="s">
         <v>29</v>
       </c>
@@ -1906,39 +2502,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" s="2" customFormat="1" spans="1:2">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" s="2" customFormat="1" spans="1:2">
       <c r="A24" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B24" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" s="2" customFormat="1" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B25" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" s="2" customFormat="1" spans="1:2">
       <c r="A26" s="2" t="s">
         <v>31</v>
       </c>
@@ -1946,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" s="2" customFormat="1" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>32</v>
       </c>
@@ -1954,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" s="2" customFormat="1" spans="1:2">
       <c r="A28" s="2" t="s">
         <v>33</v>
       </c>
@@ -1962,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" s="2" customFormat="1" spans="1:2">
       <c r="A29" s="2" t="s">
         <v>34</v>
       </c>
@@ -1970,38 +2566,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" s="2" customFormat="1" spans="1:2">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B30" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" s="2" customFormat="1" spans="1:7">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" s="2" customFormat="1" spans="1:7">
       <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
@@ -2024,39 +2620,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" s="2" customFormat="1" spans="1:2">
       <c r="A33" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="1" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" s="2" customFormat="1" spans="1:2">
       <c r="A35" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" s="2" customFormat="1" spans="1:2">
       <c r="A36" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2">
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" s="2" customFormat="1" spans="1:2">
       <c r="A37" s="2" t="s">
         <v>31</v>
       </c>
@@ -2064,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" s="2" customFormat="1" spans="1:2">
       <c r="A38" s="2" t="s">
         <v>32</v>
       </c>
@@ -2072,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" s="2" customFormat="1" spans="1:2">
       <c r="A39" s="2" t="s">
         <v>33</v>
       </c>
@@ -2080,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" s="2" customFormat="1" spans="1:2">
       <c r="A40" s="2" t="s">
         <v>34</v>
       </c>
@@ -2088,50 +2684,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" s="2" customFormat="1" spans="1:2">
       <c r="A41" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B41" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" s="2" customFormat="1" spans="1:11">
       <c r="A42" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" s="2" customFormat="1" spans="1:11">
       <c r="A43" s="2" t="s">
         <v>29</v>
       </c>
@@ -2166,39 +2762,39 @@
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" s="2" customFormat="1" spans="1:2">
       <c r="A44" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" s="1" customFormat="1" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" s="2" customFormat="1" spans="1:2">
       <c r="A46" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B46" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" s="2" customFormat="1" spans="1:2">
       <c r="A47" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B47" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" s="2" customFormat="1" spans="1:2">
       <c r="A48" s="2" t="s">
         <v>31</v>
       </c>
@@ -2206,7 +2802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" s="2" customFormat="1" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>32</v>
       </c>
@@ -2214,7 +2810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" s="2" customFormat="1" spans="1:2">
       <c r="A50" s="2" t="s">
         <v>33</v>
       </c>
@@ -2222,7 +2818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" s="2" customFormat="1" spans="1:2">
       <c r="A51" s="2" t="s">
         <v>34</v>
       </c>
@@ -2230,41 +2826,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" s="2" customFormat="1" spans="1:2">
       <c r="A52" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B52" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" s="2" customFormat="1" spans="1:8">
       <c r="A53" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" s="2" customFormat="1" spans="1:8">
       <c r="A54" s="2" t="s">
         <v>29</v>
       </c>
@@ -2290,39 +2886,39 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" s="2" customFormat="1" spans="1:2">
       <c r="A55" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" s="1" customFormat="1" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" s="2" customFormat="1" spans="1:2">
       <c r="A57" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B57" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" s="2" customFormat="1" spans="1:2">
       <c r="A58" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B58" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" s="2" customFormat="1" spans="1:2">
       <c r="A59" s="2" t="s">
         <v>31</v>
       </c>
@@ -2330,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" s="2" customFormat="1" spans="1:2">
       <c r="A60" s="2" t="s">
         <v>32</v>
       </c>
@@ -2338,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" s="2" customFormat="1" spans="1:2">
       <c r="A61" s="2" t="s">
         <v>33</v>
       </c>
@@ -2346,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" s="2" customFormat="1" spans="1:2">
       <c r="A62" s="2" t="s">
         <v>34</v>
       </c>
@@ -2354,41 +2950,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" s="2" customFormat="1" spans="1:2">
       <c r="A63" s="2" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="B63" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" s="2" customFormat="1" spans="1:8">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="65" s="2" customFormat="1" spans="1:8">
       <c r="A65" s="2" t="s">
         <v>29</v>
       </c>
@@ -2414,28 +3010,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" s="2" customFormat="1" spans="1:2">
       <c r="A66" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B19 B7:B8 D22:G30 D33:G41 A15:B17 A26:B28 A37:B39 A48:B50 A59:B61 B29:B30 A4:B6 D1:G8 B40:B41 D11:G19 B51:B52 D44:G66 B62:B63">
-      <formula1>"TRUE,FALSE"</formula1>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C8 C11:C19 C22:C30 C33:C41 C44:C66 A13:B14 A24:B25 A35:B36 A46:B47 A57:B58 A2:B3">
+      <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E42 A42:D43 F42:H43 A9:A10 A20:A21 A31:A32 A64:A65 A53:B54 L1:L19 L22:L66">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E42 A9:A10 A20:A21 A31:A32 A64:A65 L1:L19 L22:L66 A42:D43 F42:H43 A53:B54">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="I42 B9:B10 B20:B21 B31:B32 M1:M19 M22:M66"/>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:B14 A24:B25 A35:B36 A46:B47 A57:B58 C1:C8 A2:B3 C11:C19 C22:C30 C33:C41 C44:C66">
-      <formula1>0</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B8 B18:B19 B29:B30 B40:B41 B51:B52 B62:B63 D22:G30 D33:G41 A15:B17 A26:B28 A37:B39 A48:B50 A59:B61 A4:B6 D1:G8 D11:G19 D44:G66">
+      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>